<commit_message>
added a bug report
</commit_message>
<xml_diff>
--- a/дз 9-10.xlsx
+++ b/дз 9-10.xlsx
@@ -579,7 +579,7 @@
     <xdr:ext cx="3667125" cy="2886075"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image9.png" title="Изображение"/>
+        <xdr:cNvPr id="0" name="image5.png" title="Изображение"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -607,7 +607,7 @@
     <xdr:ext cx="4362450" cy="1619250"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png" title="Изображение"/>
+        <xdr:cNvPr id="0" name="image6.png" title="Изображение"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -635,7 +635,7 @@
     <xdr:ext cx="3419475" cy="1704975"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image8.png" title="Изображение"/>
+        <xdr:cNvPr id="0" name="image9.png" title="Изображение"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -719,7 +719,7 @@
     <xdr:ext cx="6419850" cy="1495425"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image6.png" title="Изображение"/>
+        <xdr:cNvPr id="0" name="image1.png" title="Изображение"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -747,7 +747,7 @@
     <xdr:ext cx="4724400" cy="3362325"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image5.png" title="Изображение"/>
+        <xdr:cNvPr id="0" name="image8.png" title="Изображение"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -775,7 +775,7 @@
     <xdr:ext cx="5438775" cy="1619250"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="Изображение"/>
+        <xdr:cNvPr id="0" name="image4.png" title="Изображение"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -831,7 +831,7 @@
     <xdr:ext cx="5829300" cy="1781175"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image4.png" title="Изображение"/>
+        <xdr:cNvPr id="0" name="image2.png" title="Изображение"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>

</xml_diff>